<commit_message>
Added xls and flatfile interactions
</commit_message>
<xml_diff>
--- a/Default.xlsx
+++ b/Default.xlsx
@@ -473,9 +473,7 @@
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>
   <cols>
@@ -511,13 +509,12 @@
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>
   <cols>
-    <col min="1" max="16384" width="9.078125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="14.2578125" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.078125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row customFormat="1"/>

</xml_diff>